<commit_message>
second version of EDA project
</commit_message>
<xml_diff>
--- a/auxiliar_data.xlsx
+++ b/auxiliar_data.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sydney\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sydney\Documents\B3. - PROJECTS\3.3. - Δ\3.3.5. - CodeUp bootcamp\3.3.5.4. - DS Bootcamp\Module 3. Exploratory Data Analysis (EDA)\EDA_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89CE26F-05B3-4DD0-BF47-C1FD98A1C48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44222D80-86EC-41EA-A405-1167514BC3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="818" activeTab="4" xr2:uid="{054ED4C8-B700-4BDD-BC37-7DF7680611CB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="818" activeTab="9" xr2:uid="{054ED4C8-B700-4BDD-BC37-7DF7680611CB}"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
     <sheet name="life" sheetId="2" r:id="rId2"/>
     <sheet name="gdp" sheetId="7" r:id="rId3"/>
     <sheet name="pop" sheetId="9" r:id="rId4"/>
-    <sheet name="life_expectancy_data" sheetId="3" r:id="rId5"/>
+    <sheet name="life_exp_data" sheetId="3" r:id="rId5"/>
     <sheet name="gdp_data" sheetId="4" r:id="rId6"/>
     <sheet name="pop_data" sheetId="6" r:id="rId7"/>
     <sheet name="lat_long_data" sheetId="8" r:id="rId8"/>
+    <sheet name="countries" sheetId="11" r:id="rId9"/>
+    <sheet name="project_str" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="286">
   <si>
     <t>rank</t>
   </si>
@@ -571,9 +573,6 @@
     <t>TCA</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
     <t>Sources</t>
   </si>
   <si>
@@ -601,9 +600,6 @@
     <t>Same as Spain</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>https://data.worldbank.org/indicator/NY.GDP.MKTP.CD</t>
   </si>
   <si>
@@ -646,13 +642,265 @@
     <t>32%2C077%20females%20and%2031%2C386%20males).</t>
   </si>
   <si>
-    <t>lat value</t>
-  </si>
-  <si>
-    <t>long value</t>
-  </si>
-  <si>
     <t>https://www.geodatos.net/en/coordinates</t>
+  </si>
+  <si>
+    <t>Part 5. Creating the definitive dataset to perform EDA.</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Addressing null values in age-related columns: `birthDate`, `birthDay`, `birthMonth` `birthYear` and `age`</t>
+  </si>
+  <si>
+    <t>Level 4</t>
+  </si>
+  <si>
+    <t>Addressing null values in `gross_tertiary_education_enrollment` and `gross_primary_education_enrollment_country`</t>
+  </si>
+  <si>
+    <t>Addressing null values in `tax_revenue_country_country` and `total_tax_rate_country`</t>
+  </si>
+  <si>
+    <t>Addressing null values in `longitude_country` and `latitude_country`</t>
+  </si>
+  <si>
+    <t>Addressing null values in `population_country` column</t>
+  </si>
+  <si>
+    <t>Addressing null values in `gdp_country` column</t>
+  </si>
+  <si>
+    <t>Addressing null values for `life_expectancy_country` column</t>
+  </si>
+  <si>
+    <t>Addressing null and missing values in country, city, and continent columns</t>
+  </si>
+  <si>
+    <t>Advanced null values addressing</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Feature engineering</t>
+  </si>
+  <si>
+    <t>Inspecting the reamining columns to look for wrong data</t>
+  </si>
+  <si>
+    <t>Looking at status and selfMade columns</t>
+  </si>
+  <si>
+    <t>Data quality inspection</t>
+  </si>
+  <si>
+    <t>Data types adjustment</t>
+  </si>
+  <si>
+    <t>Looking for duplicate values in the dataset</t>
+  </si>
+  <si>
+    <t>Part 4. Data quality improvement</t>
+  </si>
+  <si>
+    <t>Comparing category and industries columns</t>
+  </si>
+  <si>
+    <t>Part 3. Dataset structural enhancement</t>
+  </si>
+  <si>
+    <t>Addressing null values in `first_name` column</t>
+  </si>
+  <si>
+    <t>Level 5</t>
+  </si>
+  <si>
+    <t>Addressing impaired null values in `gross_tertiary_education_enrollment` and `gross_primary_education_enrollment_country`</t>
+  </si>
+  <si>
+    <t>Addressing impaired values in tax_revenue_country_country and total_tax_rate_country columns</t>
+  </si>
+  <si>
+    <t>Addressing impaired null values in cpi_country and cpi_change_country columns</t>
+  </si>
+  <si>
+    <t>Taking a look to null values in organization and title columns</t>
+  </si>
+  <si>
+    <t>Insights</t>
+  </si>
+  <si>
+    <t>Question 10. Country pop and number of billionaires. What is the frequence of being a billionaire in the Top 5 countries?</t>
+  </si>
+  <si>
+    <t>Figuring out the relation between country, state and residenceStateRegion</t>
+  </si>
+  <si>
+    <t>Question 9. What are the most common birth day, month and year for billionaires?</t>
+  </si>
+  <si>
+    <t>Dealing with null values</t>
+  </si>
+  <si>
+    <t>Question 8. Billionaires age distribution</t>
+  </si>
+  <si>
+    <t>Conducting a comparative analysis to discover influence of columns with proportion of null values</t>
+  </si>
+  <si>
+    <t>Question 7. Box plot to see the distribution of wealth across top 5 countries</t>
+  </si>
+  <si>
+    <t>Overall view of null values</t>
+  </si>
+  <si>
+    <t>Question 6. What is the overall distribution of billionaires by gender in the Top 5 countries?</t>
+  </si>
+  <si>
+    <t>Null values</t>
+  </si>
+  <si>
+    <t>Question 5. What is the most common age for billionaires?</t>
+  </si>
+  <si>
+    <t>Part 2. Data cleaning</t>
+  </si>
+  <si>
+    <t>Question 4. Which are the industries that produce the most billionaires?</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Data types and summary statistics with dtypes, info() and describe()</t>
+  </si>
+  <si>
+    <t>Question 3. How are billionaires distributed by continent and what proportion they represent?</t>
+  </si>
+  <si>
+    <t>First look at the dataset</t>
+  </si>
+  <si>
+    <t>Question 2. What are the Top 5 cities in which billionaires reside and what proportion they represent?</t>
+  </si>
+  <si>
+    <t>Setting up the environment for the project</t>
+  </si>
+  <si>
+    <t>Question 1. What are the Top 5 countries in which billionaires reside and what proportion they represent?</t>
+  </si>
+  <si>
+    <t>Part 1. Importing libraries, changing setting to display all columns and loading the dataset</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Data dictionary</t>
+  </si>
+  <si>
+    <t>Table of contents</t>
+  </si>
+  <si>
+    <t>Overview of the project</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Insights/Comments</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>32,119,15</t>
+  </si>
+  <si>
+    <t>40,152,19</t>
+  </si>
+  <si>
+    <t>51,191,24</t>
+  </si>
+  <si>
+    <t>Part 6. EDA</t>
+  </si>
+  <si>
+    <t>Basic EDA</t>
+  </si>
+  <si>
+    <t>Advanced EDA</t>
+  </si>
+  <si>
+    <t>Industry-based wealth analysis</t>
+  </si>
+  <si>
+    <t>Industry categorization</t>
+  </si>
+  <si>
+    <t>Treemap of wealth generation industries</t>
+  </si>
+  <si>
+    <t>country_name</t>
+  </si>
+  <si>
+    <t>continent</t>
+  </si>
+  <si>
+    <t>life_exp</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>Reviewed</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>lat_value</t>
+  </si>
+  <si>
+    <t>long_value</t>
+  </si>
+  <si>
+    <t>Bonus content. Spatial distribution of billionaires across the globe</t>
+  </si>
+  <si>
+    <t>Billionaires by total wealth and country</t>
+  </si>
+  <si>
+    <t>Mean and median wealth by country</t>
+  </si>
+  <si>
+    <t>Mean and median wealth by industry</t>
+  </si>
+  <si>
+    <t>Biggest and wealthiest groups by industry</t>
+  </si>
+  <si>
+    <t>Billionaires presence by industry and country</t>
+  </si>
+  <si>
+    <t>Age &amp; gender analysis</t>
+  </si>
+  <si>
+    <t>Country dashboard</t>
+  </si>
+  <si>
+    <t>Country-based wealth analysis</t>
   </si>
 </sst>
 </file>
@@ -663,7 +911,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -676,8 +924,24 @@
       <color rgb="FF3C4043"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="PT Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="PT Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="PT Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,6 +960,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF289813"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99DF8B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33BF18"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCEFC5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF20770F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -709,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -724,12 +1018,395 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF20770F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF289813"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF05BF18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99DF8B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCEFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF20770F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF289813"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF05BF18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99DF8B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCEFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF20770F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF289813"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF05BF18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99DF8B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCEFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF20770F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF289813"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF05BF18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99DF8B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCEFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF20770F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF289813"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF05BF18"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99DF8B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCEFCF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="PT Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="PT Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="PT Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="PT Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="PT Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCEFCF"/>
+      <color rgb="FF99DF8B"/>
+      <color rgb="FF05BF18"/>
+      <color rgb="FF289813"/>
+      <color rgb="FF20770F"/>
+      <color rgb="FFCCEFC5"/>
+      <color rgb="FFB4E8AA"/>
+      <color rgb="FF92DD83"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -739,6 +1416,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1EDA687E-743C-4C10-AE5C-A2B78B8F1774}" name="Table2" displayName="Table2" ref="A1:D63" totalsRowShown="0" dataDxfId="29">
+  <autoFilter ref="A1:D63" xr:uid="{4D5B8E1A-475B-4789-8AA7-8115D02364CD}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B311ADA4-5EFA-483D-B865-0773D8BC89DA}" name="Level" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{DFBA998D-CC0E-4614-842C-6F5033857235}" name="Title" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{2F5E9981-303A-4F40-95C9-55648E35B2D6}" name="Insights/Comments" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{4A056288-3512-4002-AD94-21622B6762C9}" name="Reviewed" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2024,6 +2719,876 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B113617-5785-4E01-AF7F-FF3BAA24875B}">
+  <dimension ref="A1:H63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12"/>
+  <cols>
+    <col min="2" max="2" width="40.3984375" customWidth="1"/>
+    <col min="3" max="3" width="17.59765625" customWidth="1"/>
+    <col min="8" max="8" width="19.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="H4" s="13">
+        <v>153223139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24">
+      <c r="A5" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H5" s="13">
+        <v>204239207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="24">
+      <c r="A8" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="36">
+      <c r="A12" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="24">
+      <c r="A14" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="24">
+      <c r="A15" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24">
+      <c r="A16" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="36">
+      <c r="A17" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="36">
+      <c r="A18" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="24">
+      <c r="A27" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:4" ht="24">
+      <c r="A30" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="24">
+      <c r="A31" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="24">
+      <c r="A33" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="24">
+      <c r="A34" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="36">
+      <c r="A35" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="H35" s="16"/>
+    </row>
+    <row r="36" spans="1:8" ht="36">
+      <c r="A36" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="36">
+      <c r="A37" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="24">
+      <c r="A38" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="36">
+      <c r="A41" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="36">
+      <c r="A42" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="24">
+      <c r="A43" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="24">
+      <c r="A44" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="24">
+      <c r="A45" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="24">
+      <c r="A46" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="24">
+      <c r="A47" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="24">
+      <c r="A49" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="36">
+      <c r="A50" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="24">
+      <c r="A51" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="A2:D63">
+    <cfRule type="expression" dxfId="19" priority="1">
+      <formula>$A2="Level 5"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="2">
+      <formula>$A2="Level 4"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="3">
+      <formula>$A2="Level 3"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="4">
+      <formula>$A2="Level 2"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="5">
+      <formula>$A2="Level 1"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7912BD-F6B0-4FED-A7AB-8F4C208D730C}">
   <sheetPr codeName="Sheet2"/>
@@ -3653,7 +5218,7 @@
         <v>164</v>
       </c>
       <c r="D1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E1">
         <v>1960</v>
@@ -3853,10 +5418,10 @@
         <v>166</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E2">
         <v>1320796651.6945701</v>
@@ -4056,10 +5621,10 @@
         <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E3">
         <v>1939329775.4373901</v>
@@ -4259,10 +5824,10 @@
         <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E4">
         <v>169803921.568627</v>
@@ -4462,10 +6027,10 @@
         <v>171</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E5">
         <v>84466652.588891193</v>
@@ -4665,10 +6230,10 @@
         <v>174</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E6">
         <v>35076845.969261602</v>
@@ -4868,10 +6433,10 @@
         <v>175</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AT7">
         <v>358744800</v>
@@ -4945,13 +6510,13 @@
         <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AY8">
         <v>4200288241.1529598</v>
@@ -5031,7 +6596,7 @@
         <v>164</v>
       </c>
       <c r="D1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E1">
         <v>1960</v>
@@ -5231,10 +6796,10 @@
         <v>166</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E2">
         <v>3114671</v>
@@ -5434,10 +6999,10 @@
         <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E3">
         <v>2828600</v>
@@ -5634,13 +7199,13 @@
         <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E4">
         <v>8473</v>
@@ -5840,10 +7405,10 @@
         <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E5">
         <v>114500</v>
@@ -6043,10 +7608,10 @@
         <v>171</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E6">
         <v>44400</v>
@@ -6246,10 +7811,10 @@
         <v>172</v>
       </c>
       <c r="C7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E7">
         <v>7850</v>
@@ -6449,10 +8014,10 @@
         <v>174</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E8">
         <v>345065</v>
@@ -6652,10 +8217,10 @@
         <v>175</v>
       </c>
       <c r="C9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E9">
         <v>5604</v>
@@ -6857,8 +8422,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -6869,30 +8434,30 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>269</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>176</v>
-      </c>
-      <c r="G1" t="s">
-        <v>177</v>
       </c>
       <c r="H1">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>87</v>
       </c>
       <c r="B2" s="4">
-        <v>85.492682926829303</v>
+        <v>85.5</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -6901,10 +8466,10 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
+        <v>178</v>
+      </c>
+      <c r="J2" t="s">
         <v>179</v>
-      </c>
-      <c r="J2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -6921,7 +8486,7 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6938,10 +8503,10 @@
         <v>4</v>
       </c>
       <c r="I4" t="s">
+        <v>182</v>
+      </c>
+      <c r="J4" t="s">
         <v>183</v>
-      </c>
-      <c r="J4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6949,7 +8514,7 @@
         <v>138</v>
       </c>
       <c r="B5" s="4">
-        <v>82.102439024390307</v>
+        <v>82.1</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -6968,10 +8533,10 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="B7" s="4">
-        <v>71.597999999999999</v>
+        <v>71.599999999999994</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -6982,7 +8547,7 @@
         <v>132</v>
       </c>
       <c r="B8" s="4">
-        <v>79.28</v>
+        <v>79.3</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -6996,7 +8561,7 @@
         <v>83.3</v>
       </c>
       <c r="C9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -7004,7 +8569,7 @@
         <v>134</v>
       </c>
       <c r="B10" s="4">
-        <v>74.494</v>
+        <v>74.5</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -7012,10 +8577,10 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="B11" s="4">
-        <v>57.066000000000003</v>
+        <v>57.1</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -7029,7 +8594,7 @@
         <v>81.3</v>
       </c>
       <c r="C12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -7037,7 +8602,7 @@
         <v>142</v>
       </c>
       <c r="B13" s="4">
-        <v>74.587000000000003</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -7053,42 +8618,42 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="11.796875" customWidth="1"/>
+    <col min="1" max="1" width="25.69921875" customWidth="1"/>
     <col min="2" max="2" width="15.3984375" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>267</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>186</v>
+        <v>270</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>176</v>
-      </c>
-      <c r="G1" t="s">
-        <v>177</v>
       </c>
       <c r="H1">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>87</v>
       </c>
       <c r="B2" s="5">
-        <v>368911387845.41803</v>
+        <v>368911387845</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -7097,7 +8662,7 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7114,7 +8679,7 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -7122,7 +8687,7 @@
         <v>138</v>
       </c>
       <c r="B4" s="5">
-        <v>513391778882.85999</v>
+        <v>513391778882</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -7131,7 +8696,7 @@
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -7139,7 +8704,7 @@
         <v>121</v>
       </c>
       <c r="B5" s="5">
-        <v>6028373513.49405</v>
+        <v>6028373513</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -7147,7 +8712,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="B6" s="5">
         <v>11527600000</v>
@@ -7180,10 +8745,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="B9" s="5">
-        <v>4850842571.5915098</v>
+        <v>4850842571</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -7222,37 +8787,37 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>186</v>
+        <v>271</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>176</v>
-      </c>
-      <c r="G1" t="s">
-        <v>177</v>
       </c>
       <c r="H1">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>87</v>
       </c>
       <c r="B2">
         <v>7413100</v>
@@ -7264,7 +8829,7 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -7281,10 +8846,10 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -7314,7 +8879,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="B6">
         <v>407906</v>
@@ -7347,7 +8912,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="B9">
         <v>1192271</v>
@@ -7389,7 +8954,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -7401,30 +8966,30 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>267</v>
       </c>
       <c r="B1" t="s">
-        <v>201</v>
+        <v>275</v>
       </c>
       <c r="C1" t="s">
-        <v>202</v>
+        <v>276</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>176</v>
-      </c>
-      <c r="H1" t="s">
-        <v>177</v>
       </c>
       <c r="I1">
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>87</v>
       </c>
       <c r="B2" s="6">
         <v>22.396428</v>
@@ -7489,7 +9054,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="B6" s="6">
         <v>25.034279999999999</v>
@@ -7531,7 +9096,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="B9" s="6">
         <v>-26.522503</v>
@@ -7579,10 +9144,6 @@
     </row>
     <row r="14" spans="1:10">
       <c r="H14" s="7"/>
-      <c r="I14">
-        <f>61/82</f>
-        <v>0.74390243902439024</v>
-      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="H15" s="7"/>
@@ -7591,4 +9152,655 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDD8633-4679-40CE-8C01-3F0F16693C27}">
+  <dimension ref="A1:B79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="20.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>138</v>
+      </c>
+      <c r="B46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B67" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>79</v>
+      </c>
+      <c r="B69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>142</v>
+      </c>
+      <c r="B70" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>106</v>
+      </c>
+      <c r="B73" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>109</v>
+      </c>
+      <c r="B79" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
second complete version of the project
</commit_message>
<xml_diff>
--- a/auxiliar_data.xlsx
+++ b/auxiliar_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sydney\Documents\B3. - PROJECTS\3.3. - Δ\3.3.5. - CodeUp bootcamp\3.3.5.4. - DS Bootcamp\Module 3. Exploratory Data Analysis (EDA)\EDA_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44222D80-86EC-41EA-A405-1167514BC3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15812C93-E15D-4D83-AEB1-072D077E1AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="818" activeTab="9" xr2:uid="{054ED4C8-B700-4BDD-BC37-7DF7680611CB}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="288">
   <si>
     <t>rank</t>
   </si>
@@ -901,6 +901,12 @@
   </si>
   <si>
     <t>Country-based wealth analysis</t>
+  </si>
+  <si>
+    <t>Industry dashboard</t>
+  </si>
+  <si>
+    <t>Dashboards</t>
   </si>
 </sst>
 </file>
@@ -1052,148 +1058,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF20770F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF289813"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF05BF18"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99DF8B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCEFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF20770F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF289813"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF05BF18"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99DF8B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCEFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF20770F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF289813"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF05BF18"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99DF8B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCEFCF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1419,18 +1284,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1EDA687E-743C-4C10-AE5C-A2B78B8F1774}" name="Table2" displayName="Table2" ref="A1:D63" totalsRowShown="0" dataDxfId="29">
-  <autoFilter ref="A1:D63" xr:uid="{4D5B8E1A-475B-4789-8AA7-8115D02364CD}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1EDA687E-743C-4C10-AE5C-A2B78B8F1774}" name="Table2" displayName="Table2" ref="A1:D65" totalsRowShown="0" dataDxfId="14">
+  <autoFilter ref="A1:D65" xr:uid="{4D5B8E1A-475B-4789-8AA7-8115D02364CD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B311ADA4-5EFA-483D-B865-0773D8BC89DA}" name="Level" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{DFBA998D-CC0E-4614-842C-6F5033857235}" name="Title" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{2F5E9981-303A-4F40-95C9-55648E35B2D6}" name="Insights/Comments" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{4A056288-3512-4002-AD94-21622B6762C9}" name="Reviewed" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{B311ADA4-5EFA-483D-B865-0773D8BC89DA}" name="Level" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{DFBA998D-CC0E-4614-842C-6F5033857235}" name="Title" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{2F5E9981-303A-4F40-95C9-55648E35B2D6}" name="Insights/Comments" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{4A056288-3512-4002-AD94-21622B6762C9}" name="Reviewed" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2721,11 +2586,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B113617-5785-4E01-AF7F-FF3BAA24875B}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -3511,73 +3376,93 @@
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="17" t="s">
+      <c r="A60" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="14" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C61" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D61" s="14" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="C62" s="17" t="s">
+      <c r="C62" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="14" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="17" t="s">
+      <c r="A63" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B64" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="C63" s="17"/>
-      <c r="D63" s="17"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A2:D63">
-    <cfRule type="expression" dxfId="19" priority="1">
+  <conditionalFormatting sqref="A2:D65">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A2="Level 5"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$A2="Level 4"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$A2="Level 3"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$A2="Level 2"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>$A2="Level 1"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>